<commit_message>
added the streamlit app
</commit_message>
<xml_diff>
--- a/artifacts/model_evaluation/metrics.xlsx
+++ b/artifacts/model_evaluation/metrics.xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
@@ -1335,7 +1335,6 @@
       <c r="E29" t="n">
         <v>0.01376707538052466</v>
       </c>
-      <c r="F29" t="inlineStr"/>
       <c r="G29" t="n">
         <v>0.01337260734838577</v>
       </c>
@@ -1344,6 +1343,35 @@
       </c>
       <c r="I29" t="n">
         <v>0.01571189421510127</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-12-09 09:16:46</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.9961636085978972</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.00762124003657671</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.0001757898104453401</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.01325857497792806</v>
+      </c>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="n">
+        <v>0.0130750132779512</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.0002447681723678711</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.01564506862777761</v>
       </c>
     </row>
   </sheetData>

</xml_diff>